<commit_message>
Added ICU percentage plots
</commit_message>
<xml_diff>
--- a/data/generated_summary.xlsx
+++ b/data/generated_summary.xlsx
@@ -557,13 +557,19 @@
         <v>284</v>
       </c>
       <c r="E6">
-        <v>650</v>
+        <v>588</v>
       </c>
       <c r="F6">
         <v>45</v>
       </c>
       <c r="G6">
         <v>17</v>
+      </c>
+      <c r="H6">
+        <v>650</v>
+      </c>
+      <c r="I6">
+        <v>12014</v>
       </c>
     </row>
     <row r="7" spans="1:9">

</xml_diff>

<commit_message>
Added percentage i the summary files and related plots
</commit_message>
<xml_diff>
--- a/data/generated_summary.xlsx
+++ b/data/generated_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Ricoverati con sintomi</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t>Tamponi</t>
+  </si>
+  <si>
+    <t>Percentuale deceduti su Positivi</t>
+  </si>
+  <si>
+    <t>Percentuale Guariti su Positivi</t>
+  </si>
+  <si>
+    <t>Percentuale Terpaia Intensiva su Positivi</t>
   </si>
   <si>
     <t>23.02</t>
@@ -428,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,10 +468,19 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>54</v>
@@ -482,10 +500,22 @@
       <c r="G2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="H2">
+        <v>129</v>
+      </c>
+      <c r="J2">
+        <v>1.55</v>
+      </c>
+      <c r="K2">
+        <v>0.78</v>
+      </c>
+      <c r="L2">
+        <v>20.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>101</v>
@@ -505,10 +535,22 @@
       <c r="G3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="H3">
+        <v>229</v>
+      </c>
+      <c r="J3">
+        <v>2.62</v>
+      </c>
+      <c r="K3">
+        <v>0.44</v>
+      </c>
+      <c r="L3">
+        <v>11.79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>114</v>
@@ -528,10 +570,22 @@
       <c r="G4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4">
+        <v>322</v>
+      </c>
+      <c r="J4">
+        <v>3.11</v>
+      </c>
+      <c r="K4">
+        <v>0.31</v>
+      </c>
+      <c r="L4">
+        <v>10.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>128</v>
@@ -551,10 +605,22 @@
       <c r="G5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="H5">
+        <v>400</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>0.75</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>248</v>
@@ -580,10 +646,19 @@
       <c r="I6">
         <v>12014</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>2.62</v>
+      </c>
+      <c r="K6">
+        <v>6.92</v>
+      </c>
+      <c r="L6">
+        <v>8.619999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>345</v>
@@ -609,10 +684,19 @@
       <c r="I7">
         <v>15695</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>2.36</v>
+      </c>
+      <c r="K7">
+        <v>5.18</v>
+      </c>
+      <c r="L7">
+        <v>7.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>401</v>
@@ -638,10 +722,19 @@
       <c r="I8">
         <v>18661</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>2.57</v>
+      </c>
+      <c r="K8">
+        <v>4.43</v>
+      </c>
+      <c r="L8">
+        <v>9.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>639</v>
@@ -667,10 +760,19 @@
       <c r="I9">
         <v>21127</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>2.01</v>
+      </c>
+      <c r="K9">
+        <v>4.9</v>
+      </c>
+      <c r="L9">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>742</v>
@@ -696,10 +798,19 @@
       <c r="I10">
         <v>23345</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>2.55</v>
+      </c>
+      <c r="K10">
+        <v>7.32</v>
+      </c>
+      <c r="L10">
+        <v>8.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>1034</v>
@@ -725,10 +836,19 @@
       <c r="I11">
         <v>25856</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>3.16</v>
+      </c>
+      <c r="K11">
+        <v>6.39</v>
+      </c>
+      <c r="L11">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1346</v>
@@ -753,6 +873,15 @@
       </c>
       <c r="I12">
         <v>29837</v>
+      </c>
+      <c r="J12">
+        <v>3.46</v>
+      </c>
+      <c r="K12">
+        <v>8.93</v>
+      </c>
+      <c r="L12">
+        <v>9.550000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>